<commit_message>
New USB and CWF-4 part numbers
</commit_message>
<xml_diff>
--- a/Electronics/Stepper/OUT/R2/BOM.xlsx
+++ b/Electronics/Stepper/OUT/R2/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJ\open_niryo_one\Electronics\Stepper\OUT\R2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44939B9-F90C-4DBD-9F17-7C6B8237A7FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BE3416-A3B7-44AE-BA49-44DE76657E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-1290" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="125">
   <si>
     <t>Comment</t>
   </si>
@@ -154,9 +154,6 @@
     <t>J2</t>
   </si>
   <si>
-    <t>CUI UJ2-MIBH2-4-SMT-TR</t>
-  </si>
-  <si>
     <t>Micro USB connector</t>
   </si>
   <si>
@@ -355,9 +352,6 @@
     <t>L-KLS1-207-1-02-R</t>
   </si>
   <si>
-    <t>DS1069-4 M</t>
-  </si>
-  <si>
     <t>CDRH74NP-101MC</t>
   </si>
   <si>
@@ -395,6 +389,12 @@
   </si>
   <si>
     <t>32,768 KHz cristal</t>
+  </si>
+  <si>
+    <t>TE 1981584-1</t>
+  </si>
+  <si>
+    <t>DS1069-4 MR</t>
   </si>
 </sst>
 </file>
@@ -926,7 +926,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -965,7 +965,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="1">
         <v>12</v>
@@ -982,7 +982,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -999,7 +999,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
@@ -1016,7 +1016,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1027,7 +1027,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
@@ -1050,7 +1050,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -1078,7 +1078,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>21</v>
@@ -1095,7 +1095,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>24</v>
@@ -1118,7 +1118,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -1126,14 +1126,14 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>5</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>31</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>36</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>36</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>40</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>42</v>
@@ -1259,17 +1259,17 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -1277,16 +1277,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -1294,16 +1294,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="D22" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -1311,16 +1311,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="D23" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
@@ -1328,16 +1328,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D24" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -1345,16 +1345,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -1362,16 +1362,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="D26" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" s="1">
         <v>3</v>
@@ -1379,16 +1379,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
@@ -1396,16 +1396,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D28" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1413,16 +1413,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
@@ -1430,16 +1430,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E30" s="1">
         <v>2</v>
@@ -1447,16 +1447,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D31" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
@@ -1464,16 +1464,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -1481,16 +1481,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -1498,16 +1498,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -1532,16 +1532,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="D36" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -1549,16 +1549,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -1566,16 +1566,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="D38" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -1583,16 +1583,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -1600,16 +1600,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="D40" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -1617,16 +1617,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -1634,16 +1634,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -1651,16 +1651,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
RPI hat PCB update
</commit_message>
<xml_diff>
--- a/Electronics/Stepper/OUT/R2/BOM.xlsx
+++ b/Electronics/Stepper/OUT/R2/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJ\open_niryo_one\Electronics\Stepper\OUT\R2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BE3416-A3B7-44AE-BA49-44DE76657E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8227EB9F-5941-4429-A028-651A81DA743D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-1290" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -926,7 +926,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Stepper BOM final update
</commit_message>
<xml_diff>
--- a/Electronics/Stepper/OUT/R2/BOM.xlsx
+++ b/Electronics/Stepper/OUT/R2/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJ\open_niryo_one\Electronics\Stepper\OUT\R2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8227EB9F-5941-4429-A028-651A81DA743D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461E3E32-3390-4C7C-9393-E0CF36921C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-1290" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,12 +343,6 @@
     <t>1206L200PR</t>
   </si>
   <si>
-    <t>L-KLS1-207-1-02-S</t>
-  </si>
-  <si>
-    <t>L-KLS1-207-1-04-S</t>
-  </si>
-  <si>
     <t>L-KLS1-207-1-02-R</t>
   </si>
   <si>
@@ -394,7 +388,13 @@
     <t>TE 1981584-1</t>
   </si>
   <si>
-    <t>DS1069-4 MR</t>
+    <t>5-146280-2</t>
+  </si>
+  <si>
+    <t>5-146280-4</t>
+  </si>
+  <si>
+    <t>XH2.54MM 4pins right</t>
   </si>
 </sst>
 </file>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>40</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>42</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>44</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>50</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>55</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>70</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>5</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>5</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>5</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>78</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>80</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>83</v>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>5</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>5</v>
@@ -1637,7 +1637,7 @@
         <v>91</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>92</v>
@@ -1651,10 +1651,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>94</v>

</xml_diff>